<commit_message>
Add status LEDs and update power nets
Added new 0402 LEDs (D1, D4) and supporting resistor (R12) for power-good status indication. Updated net assignments and replaced a capacitor footprint with an LED. Modified schematic and PCB files to reflect these changes.
</commit_message>
<xml_diff>
--- a/Spartan7_TriggerLogic/PSU_Stamp/Spartan7_PSU_Stamp_V0/BOM/PSU_Stamp_BOM.xlsx
+++ b/Spartan7_TriggerLogic/PSU_Stamp/Spartan7_PSU_Stamp_V0/BOM/PSU_Stamp_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Documents\IKP\HYDRA\HYDRA_VMM3_Adapter\Spartan7_TriggerLogic\PSU_Stamp\Spartan7_PSU_Stamp_V0\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4835BDA2-DDAC-4044-B22F-AE7D11664A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060C114B-FC3A-4F53-ADF2-32A5F874DD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2232" yWindow="6036" windowWidth="33960" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>LDO</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>C0805C106K8RACTU</t>
+  </si>
+  <si>
+    <t>0402 LED Green</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,6 +464,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E1" r:id="rId1" xr:uid="{867AA51F-5087-42CB-BB6B-1AC9077D4EC5}"/>

</xml_diff>

<commit_message>
Add pin header footprints and update PCB layout
Replaced C14 footprint with a pin header (J10), added new pin headers J11 and J25, and updated the PCB layout parameters. Also swapped C13 and C14 positions and made related changes to the BOM and backup files.
</commit_message>
<xml_diff>
--- a/Spartan7_TriggerLogic/PSU_Stamp/Spartan7_PSU_Stamp_V0/BOM/PSU_Stamp_BOM.xlsx
+++ b/Spartan7_TriggerLogic/PSU_Stamp/Spartan7_PSU_Stamp_V0/BOM/PSU_Stamp_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Documents\IKP\HYDRA\HYDRA_VMM3_Adapter\Spartan7_TriggerLogic\PSU_Stamp\Spartan7_PSU_Stamp_V0\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060C114B-FC3A-4F53-ADF2-32A5F874DD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637F55FA-8326-4500-A24A-324258396DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2232" yWindow="6036" windowWidth="33960" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>LDO</t>
   </si>
@@ -61,6 +61,27 @@
   </si>
   <si>
     <t>0402 LED Green</t>
+  </si>
+  <si>
+    <t>heatsink 24x24x14mm</t>
+  </si>
+  <si>
+    <t>heatsink 24x24x10mm</t>
+  </si>
+  <si>
+    <t>ATS024024014-SF-8M</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>ATS024024010-SF-8i</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Advanced-Thermal-Solutions/ATS024024014-SF-8M?qs=9vOqFld9vZUhD4gLG7MQxw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Advanced-Thermal-Solutions/ATS024024010-SF-8I?qs=9vOqFld9vZWxOh9SEW0GcA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -397,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,13 +490,49 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E1" r:id="rId1" xr:uid="{867AA51F-5087-42CB-BB6B-1AC9077D4EC5}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{6A9216EE-212E-469B-A122-E8668C6A6ED7}"/>
     <hyperlink ref="E3" r:id="rId3" xr:uid="{F042584E-8087-4C76-B5E7-3FD42641BFF4}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{A373E5FD-0BF6-487C-9FFF-9B473667C602}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{6A1B61CE-E743-4141-A4FA-27B3A8A4D025}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>